<commit_message>
Added more APIs from GT team development
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/CustomFilterList.xlsx
+++ b/BloodstreamAPI/testData/CustomFilterList.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C4FC85E7-BD0F-494D-9925-E3B72A2B8C0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18C7909-452A-41BE-BC20-051CB0928C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="19500" windowHeight="15660" tabRatio="715" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="715" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConclToApprove" sheetId="2" r:id="rId1"/>
@@ -13,9 +13,9 @@
     <sheet name="TestInfo" sheetId="4" r:id="rId3"/>
     <sheet name="WorklistDetail" sheetId="5" r:id="rId4"/>
     <sheet name="WorklistOverview" sheetId="6" r:id="rId5"/>
+    <sheet name="ArchivedSamples" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I26"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
   <si>
     <t>EndPoint</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>WorklistInformationdfsdf</t>
+  </si>
+  <si>
+    <t>ArchiveSamples</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC16E1A-EBE8-4FD7-9522-847FD03243A9}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -538,7 +544,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6AE23C-ED38-43E1-8869-59A543319E62}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -946,4 +952,106 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D68F9C-BEC4-42CE-BBFB-E7F43A50AFFD}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>